<commit_message>
Added Lumberjack and Tree sprite image to git
</commit_message>
<xml_diff>
--- a/assets/Lumberjack/Lumberjack Unit Sprite.xlsx
+++ b/assets/Lumberjack/Lumberjack Unit Sprite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="25">
   <si>
     <t>Action</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>Dimensions</t>
-  </si>
-  <si>
-    <t>128x128</t>
   </si>
   <si>
     <t>96x96</t>
@@ -450,7 +447,7 @@
   <dimension ref="A2:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -496,7 +493,7 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -514,7 +511,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -532,7 +529,7 @@
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -550,7 +547,7 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -568,7 +565,7 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
         <v>16</v>
@@ -595,7 +592,7 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" s="2"/>
     </row>
@@ -614,7 +611,7 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -638,7 +635,7 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -737,7 +734,7 @@
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -755,7 +752,7 @@
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -773,7 +770,7 @@
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -791,7 +788,7 @@
         <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -809,7 +806,7 @@
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -827,7 +824,7 @@
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -845,7 +842,7 @@
         <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -863,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:6">

</xml_diff>